<commit_message>
10.07 PMP, PSP(김지환) 수정
</commit_message>
<xml_diff>
--- a/4팀_PSP_Sheet.xlsx
+++ b/4팀_PSP_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지현\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\지환\Documents\GitHub\FiillingGood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E8888-6C5E-4D89-8EAF-6B89AB488EFD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89139E7-B072-47F5-94A5-226EF87700CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="1635" windowWidth="21150" windowHeight="16530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="총합" sheetId="1" r:id="rId1"/>
@@ -1219,7 +1219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1264,10 +1264,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>빵끝</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>김동욱</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1300,10 +1296,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>filling-good</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Use Case Outline </t>
     </r>
@@ -1318,6 +1310,111 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>FillingGood</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.09.25</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UseCase Diagram 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.09.27</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.09.28</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Outline </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>담당 파트 작성</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.10.04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Outline </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성 토의 및 각 기능별 역할 분담</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UseCase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성 관련 토의</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.10.07</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UseCase Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>담당부분 작성 및 전체 수정 취합</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1327,7 +1424,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1404,6 +1501,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
     </font>
@@ -1883,19 +1986,19 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.85" customHeight="1">
+    <row r="1" spans="1:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1907,23 +2010,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.85" customHeight="1">
+    <row r="2" spans="1:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.85" customHeight="1"/>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26.4">
+    <row r="4" spans="1:6" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +2046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1951,7 +2054,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1959,7 +2062,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1967,7 +2070,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1975,7 +2078,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1983,7 +2086,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1991,7 +2094,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1999,7 +2102,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2007,7 +2110,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2015,7 +2118,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2023,7 +2126,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2031,7 +2134,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2039,7 +2142,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2047,7 +2150,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2055,7 +2158,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2063,7 +2166,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2071,7 +2174,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2079,7 +2182,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2087,7 +2190,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2095,7 +2198,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2103,7 +2206,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2111,7 +2214,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2119,7 +2222,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2127,7 +2230,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2135,7 +2238,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2143,7 +2246,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2151,7 +2254,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2159,7 +2262,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2167,7 +2270,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2175,7 +2278,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2183,7 +2286,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2191,7 +2294,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2199,7 +2302,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2224,7 +2327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2241,7 +2344,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2258,7 +2361,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2275,7 +2378,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2292,7 +2395,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2309,7 +2412,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2326,7 +2429,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2343,16 +2446,16 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="49.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2364,30 +2467,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2415,7 +2518,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2423,7 +2526,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2431,7 +2534,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2439,7 +2542,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2447,7 +2550,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2455,7 +2558,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2463,7 +2566,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2471,7 +2574,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2479,7 +2582,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2487,7 +2590,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2495,7 +2598,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2503,7 +2606,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2511,7 +2614,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2519,7 +2622,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2527,7 +2630,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2535,7 +2638,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2543,7 +2646,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2551,7 +2654,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2559,7 +2662,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2567,7 +2670,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2575,7 +2678,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2583,7 +2686,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2591,7 +2694,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2599,7 +2702,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2607,7 +2710,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2615,7 +2718,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2623,7 +2726,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2631,7 +2734,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2639,7 +2742,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2647,7 +2750,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2655,7 +2758,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2663,7 +2766,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2686,17 +2789,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2708,12 +2811,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -2724,14 +2827,14 @@
         <v>8</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2751,9 +2854,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>8.3333333333333329E-2</v>
@@ -2766,12 +2869,12 @@
         <v>60</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>0.3125</v>
@@ -2784,10 +2887,10 @@
         <v>60</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2795,7 +2898,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2803,7 +2906,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2811,7 +2914,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2819,7 +2922,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2827,7 +2930,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2835,7 +2938,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2843,7 +2946,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2851,7 +2954,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2859,7 +2962,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2867,7 +2970,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2875,7 +2978,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2883,7 +2986,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2891,7 +2994,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2899,7 +3002,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2907,7 +3010,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2915,7 +3018,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2923,7 +3026,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2931,7 +3034,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2939,7 +3042,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2947,7 +3050,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2955,7 +3058,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2963,7 +3066,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2971,7 +3074,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2979,7 +3082,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2987,7 +3090,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2995,7 +3098,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3003,7 +3106,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3011,7 +3114,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3019,7 +3122,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3027,7 +3130,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3050,17 +3153,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3072,30 +3175,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3115,47 +3218,107 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
-      <c r="A6" s="13"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="13"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>40</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0347222222222221</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>130</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3163,7 +3326,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3171,7 +3334,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3179,7 +3342,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3187,7 +3350,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3195,7 +3358,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3203,7 +3366,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3211,7 +3374,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3219,7 +3382,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3227,7 +3390,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3235,7 +3398,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3243,7 +3406,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3251,7 +3414,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3259,7 +3422,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3267,7 +3430,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3275,7 +3438,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3283,7 +3446,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3291,7 +3454,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3299,7 +3462,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3307,7 +3470,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3315,7 +3478,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3323,7 +3486,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3331,7 +3494,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3339,7 +3502,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3347,7 +3510,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3355,7 +3518,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3363,7 +3526,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3371,7 +3534,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3382,11 +3545,12 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3395,16 +3559,16 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3416,30 +3580,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3459,7 +3623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3467,7 +3631,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3475,7 +3639,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3483,7 +3647,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3491,7 +3655,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3499,7 +3663,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3507,7 +3671,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3515,7 +3679,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3523,7 +3687,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3531,7 +3695,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3539,7 +3703,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3547,7 +3711,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3555,7 +3719,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3563,7 +3727,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3571,7 +3735,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3579,7 +3743,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3587,7 +3751,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3595,7 +3759,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3603,7 +3767,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3611,7 +3775,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3619,7 +3783,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3627,7 +3791,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3635,7 +3799,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3643,7 +3807,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3651,7 +3815,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3659,7 +3823,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3667,7 +3831,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3675,7 +3839,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3683,7 +3847,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3691,7 +3855,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3699,7 +3863,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3707,7 +3871,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3715,7 +3879,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3739,16 +3903,16 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3760,30 +3924,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="13.8">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3803,7 +3967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3811,7 +3975,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3819,7 +3983,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3827,7 +3991,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3835,7 +3999,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3843,7 +4007,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3851,7 +4015,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3859,7 +4023,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3867,7 +4031,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3875,7 +4039,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3883,7 +4047,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3891,7 +4055,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3899,7 +4063,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="13.8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3907,7 +4071,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3915,7 +4079,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3923,7 +4087,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="13.8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3931,7 +4095,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3939,7 +4103,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3947,7 +4111,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3955,7 +4119,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3963,7 +4127,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3971,7 +4135,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3979,7 +4143,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3987,7 +4151,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3995,7 +4159,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4003,7 +4167,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4011,7 +4175,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4019,7 +4183,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4027,7 +4191,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4035,7 +4199,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4043,7 +4207,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4051,7 +4215,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4059,7 +4223,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4084,7 +4248,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4101,7 +4265,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4118,7 +4282,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>